<commit_message>
updated in order to be aligned with importers file
It is the same that this one
https://github.com/landportal/landbook-importers/blob/32f5f0a749d574b94a53910d565498f60a173d9d/CountryReconciler/reconciler/files/country_list.xlsx
</commit_message>
<xml_diff>
--- a/countries/country_list.xlsx
+++ b/countries/country_list.xlsx
@@ -6651,7 +6651,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -6758,6 +6758,12 @@
       <sz val="10"/>
       <color theme="11"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="19">
@@ -7165,7 +7171,7 @@
     <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="147">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -7790,6 +7796,150 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1104900</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12696825" cy="12849225"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1104900</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12696825" cy="12849225"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1104900</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12696825" cy="12849225"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8082,8 +8232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B176" workbookViewId="0">
-      <selection activeCell="D185" sqref="D185"/>
+    <sheetView tabSelected="1" topLeftCell="AQ74" workbookViewId="0">
+      <selection activeCell="AV103" sqref="AV103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -20911,7 +21061,9 @@
       <c r="AU90" s="7">
         <v>-99</v>
       </c>
-      <c r="AV90" s="24"/>
+      <c r="AV90" s="24">
+        <v>85</v>
+      </c>
     </row>
     <row r="91" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A91" s="17" t="s">
@@ -22550,7 +22702,9 @@
       <c r="AU102" s="7">
         <v>-99</v>
       </c>
-      <c r="AV102" s="24"/>
+      <c r="AV102" s="24">
+        <v>264</v>
+      </c>
     </row>
     <row r="103" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A103" s="17" t="s">
@@ -29720,7 +29874,9 @@
       <c r="AU152" s="7">
         <v>-99</v>
       </c>
-      <c r="AV152" s="24"/>
+      <c r="AV152" s="24">
+        <v>163</v>
+      </c>
     </row>
     <row r="153" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A153" s="17" t="s">
@@ -31224,7 +31380,9 @@
       <c r="AU163" s="7">
         <v>-99</v>
       </c>
-      <c r="AV163" s="24"/>
+      <c r="AV163" s="24">
+        <v>161</v>
+      </c>
     </row>
     <row r="164" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A164" s="17" t="s">
@@ -32948,7 +33106,9 @@
       <c r="AU175" s="7">
         <v>-99</v>
       </c>
-      <c r="AV175" s="24"/>
+      <c r="AV175" s="24">
+        <v>172</v>
+      </c>
     </row>
     <row r="176" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A176" s="17" t="s">
@@ -35312,7 +35472,9 @@
       <c r="AU192" s="7">
         <v>1</v>
       </c>
-      <c r="AV192" s="24"/>
+      <c r="AV192" s="24">
+        <v>205</v>
+      </c>
     </row>
     <row r="193" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A193" s="17" t="s">
@@ -40550,6 +40712,9 @@
       <c r="AU229" s="17">
         <v>1</v>
       </c>
+      <c r="AV229">
+        <v>227</v>
+      </c>
     </row>
     <row r="230" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A230" s="17" t="s">
@@ -42129,7 +42294,9 @@
       <c r="AU240" s="7">
         <v>-99</v>
       </c>
-      <c r="AV240" s="24"/>
+      <c r="AV240" s="24">
+        <v>240</v>
+      </c>
     </row>
     <row r="241" spans="1:48" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A241" s="17" t="s">
@@ -43879,9 +44046,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Added Kosovo as country
</commit_message>
<xml_diff>
--- a/countries/country_list.xlsx
+++ b/countries/country_list.xlsx
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9316" uniqueCount="2227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9325" uniqueCount="2230">
   <si>
     <t>sovereignt,C,254</t>
   </si>
@@ -6763,6 +6763,15 @@
   </si>
   <si>
     <t>alternative EN name 1</t>
+  </si>
+  <si>
+    <t>XKX</t>
+  </si>
+  <si>
+    <t>Kosovo</t>
+  </si>
+  <si>
+    <t>XK</t>
   </si>
 </sst>
 </file>
@@ -7655,7 +7664,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="24" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -7823,6 +7832,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="152" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="43" fillId="0" borderId="0" xfId="152" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="20" borderId="0" xfId="154" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="20" borderId="0" xfId="154" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -9405,10 +9420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K250"/>
+  <dimension ref="A1:K251"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A214" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C233" sqref="C233"/>
+    <sheetView tabSelected="1" topLeftCell="A215" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D236" sqref="D236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -18168,6 +18183,35 @@
       </c>
       <c r="K250" s="67" t="s">
         <v>81</v>
+      </c>
+    </row>
+    <row r="251" spans="1:11" s="77" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A251" s="77" t="s">
+        <v>2227</v>
+      </c>
+      <c r="B251" s="77" t="s">
+        <v>2228</v>
+      </c>
+      <c r="C251" s="77" t="s">
+        <v>2228</v>
+      </c>
+      <c r="D251" s="77" t="s">
+        <v>2228</v>
+      </c>
+      <c r="E251" s="77" t="s">
+        <v>2228</v>
+      </c>
+      <c r="F251" s="77" t="s">
+        <v>2228</v>
+      </c>
+      <c r="G251" s="77" t="s">
+        <v>2228</v>
+      </c>
+      <c r="H251" s="77" t="s">
+        <v>2229</v>
+      </c>
+      <c r="K251" s="78" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>